<commit_message>
Added some boilerplate for particle sims, towards rendering next
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FF6236-D6D8-40BB-B438-FB01BBF49E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3DA616-8106-4DC2-848A-4B7EB8FA3C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="3630" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>PVM</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>Kirjan sivut 1-35, orientaatio &amp; vektorit</t>
+  </si>
+  <si>
+    <t>26 syys</t>
+  </si>
+  <si>
+    <t>Kirjan sivut 36-54</t>
+  </si>
+  <si>
+    <t>12.00-13:30, 13:45-14:15</t>
+  </si>
+  <si>
+    <t>Pieniä viilauksia koodiin ja projektirakenteeseen esim headerit, ja nimiavaruuksien kertailua sekä konstruktorien otsaketiedosto sekä toteuttava luokka</t>
+  </si>
+  <si>
+    <t>Huonot yöunet verottivat mutta välillä kun nousi ylös niin pysyi hereillä. Motivaatio korkealla edelleen saada jotain ruudulle myös näkymään, pientä lämmittelyä nämä pari päivää.</t>
   </si>
 </sst>
 </file>
@@ -401,9 +416,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -466,7 +481,27 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>2.5</v>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still working on renderable sphere as renderableparticle
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3DA616-8106-4DC2-848A-4B7EB8FA3C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD025D5-4916-4D8C-9B4C-C8E2F0C79D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="3630" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>PVM</t>
   </si>
@@ -80,9 +80,6 @@
     <t>26 syys</t>
   </si>
   <si>
-    <t>Kirjan sivut 36-54</t>
-  </si>
-  <si>
     <t>12.00-13:30, 13:45-14:15</t>
   </si>
   <si>
@@ -90,6 +87,18 @@
   </si>
   <si>
     <t>Huonot yöunet verottivat mutta välillä kun nousi ylös niin pysyi hereillä. Motivaatio korkealla edelleen saada jotain ruudulle myös näkymään, pientä lämmittelyä nämä pari päivää.</t>
+  </si>
+  <si>
+    <t>29 syys</t>
+  </si>
+  <si>
+    <t>Kirjan sivut 36-54, calculuksen pikakertausta ja johdantoa partikkeleihin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>9.00-10.45</t>
   </si>
 </sst>
 </file>
@@ -125,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -136,6 +145,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +491,7 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -489,19 +499,35 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scene boilerplate, need a shader next
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD025D5-4916-4D8C-9B4C-C8E2F0C79D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CBCBAC-09FF-45EF-843D-D806BDDD08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="3630" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>9.00-10.45</t>
+    <t>9.00-10.45, 11:45-13.00</t>
   </si>
 </sst>
 </file>
@@ -134,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -145,7 +145,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +428,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,11 +513,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G5">

</xml_diff>

<commit_message>
Discovered source of error : typo in file paths
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1243905-F918-465E-B13B-127F4160A4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C204BDC-73B1-456A-B137-B98AD7BB8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3970" yWindow="3630" windowWidth="26930" windowHeight="14950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8610" yWindow="3920" windowWidth="26930" windowHeight="14950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>PVM</t>
   </si>
@@ -98,9 +98,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>9.00-10.45, 11:45-13.00, 14.00-16.00</t>
-  </si>
-  <si>
     <t>Partikkelin pähkäilyä ruudulle, pallon renderöinti alkutekijöistä, projektirakenteen pähkäilyä ja kirjastojen linkkailua</t>
   </si>
   <si>
@@ -108,6 +105,27 @@
   </si>
   <si>
     <t>Tänään syntyi aika paljon koodia, mutta osa samaa boilerplatea RR kurssilta. Kyllä aika monta riviä saa olla, ennenkuin saa mitään näkymään, toivottavasti huomenan näin käy.</t>
+  </si>
+  <si>
+    <t>1 loka</t>
+  </si>
+  <si>
+    <t>Eli näköjään kun käyttä glad, ja glfw tai muuta kirjastoa, tulee aina ensin sisällyttää glad, riippumatta tarvitseeko sitä ko tiedostossa. Tällöin vältytään include guard virheeltä joka tulkitsee gl.h kirjaston sisällyttämisen kahdesti.</t>
+  </si>
+  <si>
+    <t>Edelleen partikkelia yritän saada näkymään. Projektirakenteen siistimistä, C++ syntaksin ihmettelyä.</t>
+  </si>
+  <si>
+    <t>Pakko sanoa, että luulin jo päässeeni sinuiksi enemmän tällaisten aloittelijan virheiden kanssa, mutta se on hyvä opettaja kun koodi ei toimi. Täytyy huolehtia, että jää aikaa opetella myös asiasisältöä, mutta tässä toistaiseksi ollut ihan hommaa että saa omat solmut availtua.</t>
+  </si>
+  <si>
+    <t>Oppiminen olisi tehokkaampaa, jos olisi enemmän sujut kielen kanssa. Kyllä tämä tästä jossakin vaiheessa.</t>
+  </si>
+  <si>
+    <t>9.00-10.45, 11:45-13.00, 14.00-15.00</t>
+  </si>
+  <si>
+    <t>17.50-18.50, 19.15-20.45</t>
   </si>
 </sst>
 </file>
@@ -437,7 +455,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,8 +465,8 @@
     <col min="3" max="3" width="29.453125" customWidth="1"/>
     <col min="4" max="4" width="41.36328125" customWidth="1"/>
     <col min="5" max="5" width="34.6328125" customWidth="1"/>
-    <col min="6" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="6" max="6" width="32.36328125" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
     <col min="8" max="8" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,7 +517,7 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>9.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -527,19 +545,42 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="G5">
-        <v>5</v>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
no rendered particles, all desired functions get called
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C204BDC-73B1-456A-B137-B98AD7BB8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADB785E-B3F1-4EE2-8197-CC1F16C377D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8610" yWindow="3920" windowWidth="26930" windowHeight="14950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10610" yWindow="3970" windowWidth="26930" windowHeight="14950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>PVM</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>17.50-18.50, 19.15-20.45</t>
+  </si>
+  <si>
+    <t>6 loka</t>
+  </si>
+  <si>
+    <t>Nyt löytyi tuo virhe miksei näy mitään ruudulla tai oikeastaan miksei varjostimet käänny, laitetaan alustajalistalla merkkijonomuuttujien väliin se pilkku eikä sinne sisälle</t>
+  </si>
+  <si>
+    <t>11.45-13:15, 13:30-15:00</t>
+  </si>
+  <si>
+    <t>Partikkelidemon pohjustelua</t>
   </si>
 </sst>
 </file>
@@ -161,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,6 +184,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +468,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +596,19 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Working on grid, OpenGL gets rid of uniforms annoyingly
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C59A377-09ED-4695-89E5-1F4057238BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D509CEC-552C-43F0-B762-8D7044B5FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="3700" windowWidth="22600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18250" yWindow="5640" windowWidth="19770" windowHeight="13910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>PVM</t>
   </si>
@@ -174,6 +174,27 @@
   </si>
   <si>
     <t>Nooh, mitä tähän nyt sanoisi. Tuntuu, että aikaa verottaa tuo työkalujen kanssa tappelu. Fiilis on, että ehkä ennen kurssia olisi pitänyt puuhastella omaa ajatusmaailmaa ja taitotasoa kuntoon. Mutta tällä  mennään.</t>
+  </si>
+  <si>
+    <t>19 loka</t>
+  </si>
+  <si>
+    <t>18.30-21.00</t>
+  </si>
+  <si>
+    <t>Kameraluokka, liikkuminen scenessä ja ruudukko</t>
+  </si>
+  <si>
+    <t>Alussa vaikutti olevan hyvä meininki mutta jumiin jäätiin. Näyttää olevan kantava teema.</t>
+  </si>
+  <si>
+    <t>Kyllähän tämä tästä, hieman siistimmin taas muutama asia opittu kuten compile time constant eli constexpr jota käytettiin kameran alustuksessa.</t>
+  </si>
+  <si>
+    <t>20 loka</t>
+  </si>
+  <si>
+    <t>20.30-21.30</t>
   </si>
 </sst>
 </file>
@@ -501,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,7 +587,7 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>18.75</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -698,9 +719,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="6"/>
-      <c r="C10" s="2"/>
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small work on scene
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D509CEC-552C-43F0-B762-8D7044B5FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD58CD66-81F9-4AB4-922E-5D2A7F2AF1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18250" yWindow="5640" windowWidth="19770" windowHeight="13910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15220" yWindow="4990" windowWidth="19770" windowHeight="13910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>PVM</t>
   </si>
@@ -182,9 +182,6 @@
     <t>18.30-21.00</t>
   </si>
   <si>
-    <t>Kameraluokka, liikkuminen scenessä ja ruudukko</t>
-  </si>
-  <si>
     <t>Alussa vaikutti olevan hyvä meininki mutta jumiin jäätiin. Näyttää olevan kantava teema.</t>
   </si>
   <si>
@@ -195,6 +192,18 @@
   </si>
   <si>
     <t>20.30-21.30</t>
+  </si>
+  <si>
+    <t>21 loka</t>
+  </si>
+  <si>
+    <t>Kameraluokka, liikkuminen scenessä</t>
+  </si>
+  <si>
+    <t>Infinite grid tutoriaalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.15-10.15, 14.00-17.00, </t>
   </si>
 </sst>
 </file>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -727,13 +736,13 @@
         <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="G10">
         <v>2.5</v>
@@ -741,10 +750,21 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>52</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small update on camera
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD58CD66-81F9-4AB4-922E-5D2A7F2AF1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAE7BCE-72CA-4263-806B-13B8689B4B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="4990" windowWidth="19770" windowHeight="13910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13500" yWindow="3290" windowWidth="19770" windowHeight="13910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>PVM</t>
   </si>
@@ -203,7 +203,19 @@
     <t>Infinite grid tutoriaalia</t>
   </si>
   <si>
-    <t xml:space="preserve">9.15-10.15, 14.00-17.00, </t>
+    <t>Infinite grid yritelmää</t>
+  </si>
+  <si>
+    <t>Aikalailla täysi nolla, kunnes tajusin että niin, klippaushan siinä tapahtuu. Kaikkia tunteja ei ole viitsitty kirjata kun eivät olleet tehokkaita.</t>
+  </si>
+  <si>
+    <t>Tuli pientä sörkkimistä joka puolelta debug mielessä, mutta periaatteisiinhan se kosahti. Near - plane oli liian lähellä, ja pieni "hack" joka nosti y tasoa hieman selitti enemmän kuin haluan myöntää.</t>
+  </si>
+  <si>
+    <t>9.15-10.30, 14.00-17.00, 19.00-19.45</t>
+  </si>
+  <si>
+    <t>Täytyy alkaa pohtia jos alkaa oikeasti mennä näin kauan aikaa "perustan" parantamiseen ja openGL kikkailuihin, onko mielekästä kurssia tässä kohtaa yrittää käydä? Priorisoidaan, ja onhan tässä 10 viikkoa. Toivottavasti pian päästään kirjassakin eteenpäin.</t>
   </si>
 </sst>
 </file>
@@ -533,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,7 +608,7 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>21.25</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -759,12 +771,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working towards working split of firework, firework rules and fireworks scene
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BA5937-6BA4-4001-BA86-BA16404A5A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22208E9-79F4-4B51-BE6B-C1F3E2ED0803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12550" yWindow="3010" windowWidth="25530" windowHeight="17870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12750" yWindow="2770" windowWidth="25530" windowHeight="17870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>PVM</t>
   </si>
@@ -246,6 +246,21 @@
   </si>
   <si>
     <t>Yrityksenä hieman modernisoida esimerkkimoottorin koodikantaa ja tehdä siitä oman näköistä, katsotaan mitä tapahtuu</t>
+  </si>
+  <si>
+    <t>24 loka</t>
+  </si>
+  <si>
+    <t>14.45-16.00, 17.15-18.30</t>
+  </si>
+  <si>
+    <t>Firework puuhat jatkuivat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modernisoinnissa haastetta, ehkä pitäisi ensi kerralla enemmän kopioida esimerkkimoottorista asioita, ja sitten pikkuhiljaa muutella mutta nyt pitää mennä tällä. </t>
+  </si>
+  <si>
+    <t>Ok, ihan hyvä meininki. Toisten koodin tutkimisestakin oppii paljon ja sitäkin pitää työelämää varten paljon tehdä.</t>
   </si>
 </sst>
 </file>
@@ -573,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,7 +653,7 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>30.25</v>
+        <v>32.75</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -862,6 +877,26 @@
       </c>
       <c r="G14">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert to previous camera default
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22208E9-79F4-4B51-BE6B-C1F3E2ED0803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983466F8-308B-425F-96C3-BAFC4FDC0BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12750" yWindow="2770" windowWidth="25530" windowHeight="17870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="190" yWindow="0" windowWidth="38300" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>PVM</t>
   </si>
@@ -261,6 +261,24 @@
   </si>
   <si>
     <t>Ok, ihan hyvä meininki. Toisten koodin tutkimisestakin oppii paljon ja sitäkin pitää työelämää varten paljon tehdä.</t>
+  </si>
+  <si>
+    <t>27 loka</t>
+  </si>
+  <si>
+    <t>Fireworkit näkymään modernimmalla c++, pikakurssi C++ iteraattoreihin tekoälyn johdolla, pikakertaus OpenGL primitiiveihin</t>
+  </si>
+  <si>
+    <t>12.45-15.15, 16.15-17.15, 18.15-20.15, 20.30-21.00</t>
+  </si>
+  <si>
+    <t>Koodistakin alkaa löytyä vähän järkeä, kun sai tuon uniformin käytettyä uudestaan firework scenessä. Nyt on oikeasti hyvä fiilis jatkaa eteenpäin, kun sai kaiken toimimaan ja hieman modernimmalla c++:lla. Aika hakusessahan tuo vielä on, ja virheen löytäminen on työn ja tuskan takana.</t>
+  </si>
+  <si>
+    <t>Tästä jatketaan kohti kytkettyjä kappaleita!</t>
+  </si>
+  <si>
+    <t>No, siellä 80-90% mentiin, ei voi ymmärtää mitä ei ymmärrä ja tässä haasteena on modernisoida koodikantaa mitä ei kunnolla ymmärrä, eikä sitä modernisointiakaan vielä hanskaa. Taistelu kerrallaan toivon mukaan kehittyy myös tässä</t>
   </si>
 </sst>
 </file>
@@ -588,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,7 +671,7 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(G3:G40)</f>
-        <v>32.75</v>
+        <v>38.75</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -898,6 +916,32 @@
       <c r="G15">
         <v>2.5</v>
       </c>
+    </row>
+    <row r="16" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
learning diary + ideal stiff spring forcegenerator
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983466F8-308B-425F-96C3-BAFC4FDC0BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCC6915-2548-4091-B8F9-AF71BE07D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="190" yWindow="0" windowWidth="38300" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="38300" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>PVM</t>
   </si>
@@ -164,9 +164,6 @@
     <t>13 loka</t>
   </si>
   <si>
-    <t>18.00-20.15</t>
-  </si>
-  <si>
     <t>Koodikannan uudelleenorganisointi järkevämmäksi, scene.cpp ideointi ja täydennys.</t>
   </si>
   <si>
@@ -279,6 +276,24 @@
   </si>
   <si>
     <t>No, siellä 80-90% mentiin, ei voi ymmärtää mitä ei ymmärrä ja tässä haasteena on modernisoida koodikantaa mitä ei kunnolla ymmärrä, eikä sitä modernisointiakaan vielä hanskaa. Taistelu kerrallaan toivon mukaan kehittyy myös tässä</t>
+  </si>
+  <si>
+    <t>28 loka</t>
+  </si>
+  <si>
+    <t>D'Alamembertin laki, Hookin laki, Oppikirjasta 79-103</t>
+  </si>
+  <si>
+    <t>8.45-10.45, 11.45-13.15</t>
+  </si>
+  <si>
+    <t>Noniin, nyt roppakaupalla uutta asiaa. Kirja on aika hyvä, siellä pedataan paljon että miksi asiat tehdään sillä tavalla ja mitä jatkossa luvassa.</t>
+  </si>
+  <si>
+    <t>Katsotaan mitä modernisointia tähän demoon löytyy, nyt kopioitu lähinnä boilerplatea. Ehkä huomenna koodaillaan enemmän.</t>
+  </si>
+  <si>
+    <t>18.00-20.30</t>
   </si>
 </sst>
 </file>
@@ -314,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -324,7 +339,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -609,7 +623,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,7 +635,7 @@
     <col min="5" max="5" width="34.6328125" customWidth="1"/>
     <col min="6" max="6" width="32.36328125" customWidth="1"/>
     <col min="7" max="7" width="15.1796875" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -669,9 +683,9 @@
       <c r="G3" s="4">
         <v>2.5</v>
       </c>
-      <c r="H3" s="5">
-        <f>SUM(G3:G40)</f>
-        <v>38.75</v>
+      <c r="H3" s="4">
+        <f>SUM(G3:G60)</f>
+        <v>43.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -764,7 +778,7 @@
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -787,37 +801,37 @@
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G9">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="G10">
         <v>2.5</v>
@@ -825,33 +839,36 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="G12">
         <v>5</v>
@@ -859,19 +876,19 @@
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="G13">
         <v>2.5</v>
@@ -879,19 +896,19 @@
     </row>
     <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="G14">
         <v>1.5</v>
@@ -899,19 +916,19 @@
     </row>
     <row r="15" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="G15">
         <v>2.5</v>
@@ -919,29 +936,46 @@
     </row>
     <row r="16" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First aggregate demo skeleton in plac
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCC6915-2548-4091-B8F9-AF71BE07D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783C495A-F7B1-4A55-9038-01F7009D0402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="0" windowWidth="38300" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>PVM</t>
   </si>
@@ -284,9 +284,6 @@
     <t>D'Alamembertin laki, Hookin laki, Oppikirjasta 79-103</t>
   </si>
   <si>
-    <t>8.45-10.45, 11.45-13.15</t>
-  </si>
-  <si>
     <t>Noniin, nyt roppakaupalla uutta asiaa. Kirja on aika hyvä, siellä pedataan paljon että miksi asiat tehdään sillä tavalla ja mitä jatkossa luvassa.</t>
   </si>
   <si>
@@ -294,6 +291,24 @@
   </si>
   <si>
     <t>18.00-20.30</t>
+  </si>
+  <si>
+    <t>ImGui integrointi iltapuhteena, tästä tulee hyvä</t>
+  </si>
+  <si>
+    <t>8.45-10.45, 11.45-13.15, 19.45-20.45</t>
+  </si>
+  <si>
+    <t>29 loka</t>
+  </si>
+  <si>
+    <t>Kytketyn kappaleen demoa</t>
+  </si>
+  <si>
+    <t>19.15-21.45</t>
+  </si>
+  <si>
+    <t>Jospa nyt olisi se particle.cpp integrointi metodi kunnossa :D . Vielä pitää korjata firework, mutta eka kytketty kappale demo pohja valmiina.</t>
   </si>
 </sst>
 </file>
@@ -620,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +700,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>43.5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -802,7 +817,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
@@ -962,19 +977,39 @@
         <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>84</v>
+      <c r="F17" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G17">
-        <v>3.5</v>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pulling mutable state from scenes to renderer
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783C495A-F7B1-4A55-9038-01F7009D0402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF95D29-ED6D-406A-B710-90FC11BCEF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="0" windowWidth="38300" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>PVM</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>Jospa nyt olisi se particle.cpp integrointi metodi kunnossa :D . Vielä pitää korjata firework, mutta eka kytketty kappale demo pohja valmiina.</t>
+  </si>
+  <si>
+    <t>30 loka</t>
+  </si>
+  <si>
+    <t>9.15-11.15</t>
+  </si>
+  <si>
+    <t>Initial draw ongelman selvittelyä fireworkscenestä, oppikirjasta 104-</t>
   </si>
 </sst>
 </file>
@@ -635,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,7 +709,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1010,6 +1019,20 @@
       </c>
       <c r="G18">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all initial rendering issues fixed, stable build
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF95D29-ED6D-406A-B710-90FC11BCEF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA94A37-7D02-4959-8043-A1F637E33CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="0" windowWidth="38300" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>PVM</t>
   </si>
@@ -314,10 +314,19 @@
     <t>30 loka</t>
   </si>
   <si>
-    <t>9.15-11.15</t>
-  </si>
-  <si>
-    <t>Initial draw ongelman selvittelyä fireworkscenestä, oppikirjasta 104-</t>
+    <t>Initial draw ongelman selvittelyä fireworkscenestä</t>
+  </si>
+  <si>
+    <t>9.15-11.15, 20.15-22.15</t>
+  </si>
+  <si>
+    <t>Vedetty muuttuvaa tilaa yhteen paikkaan ja oiottu skeneä hieman.</t>
+  </si>
+  <si>
+    <t>noh tulipa sentään korjattua initial draw ongelmaa aika järeästi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kyllä tähän voisi melkein tottua että saa asioita aikaan</t>
   </si>
 </sst>
 </file>
@@ -646,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,7 +718,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1021,18 +1030,27 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>93</v>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Particle contact base resolution algos
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA94A37-7D02-4959-8043-A1F637E33CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EDCF80-1550-4040-8557-0CB9D0037DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="38300" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>PVM</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Kyllä tähän voisi melkein tottua että saa asioita aikaan</t>
+  </si>
+  <si>
+    <t>31 loka</t>
+  </si>
+  <si>
+    <t>12.00-13.00, 16.45-</t>
+  </si>
+  <si>
+    <t>Tsempring, rajoitteet kytketyissä kappaleissa</t>
   </si>
 </sst>
 </file>
@@ -653,20 +662,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="29.453125" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" customWidth="1"/>
-    <col min="6" max="6" width="32.36328125" customWidth="1"/>
+    <col min="4" max="4" width="41.453125" customWidth="1"/>
+    <col min="5" max="5" width="34.54296875" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
     <col min="7" max="7" width="15.1796875" customWidth="1"/>
     <col min="8" max="8" width="10.26953125" customWidth="1"/>
   </cols>
@@ -1046,11 +1055,22 @@
       <c r="E19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>96</v>
       </c>
       <c r="G19">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resting contact resolution for ptcls
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EDCF80-1550-4040-8557-0CB9D0037DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02072C9-A235-4140-9F14-BA934604754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,10 +332,10 @@
     <t>31 loka</t>
   </si>
   <si>
-    <t>12.00-13.00, 16.45-</t>
-  </si>
-  <si>
     <t>Tsempring, rajoitteet kytketyissä kappaleissa</t>
+  </si>
+  <si>
+    <t>12.00-13.00, 16.45-17.45,</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1067,10 +1067,10 @@
         <v>97</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complemented mass-agregate engine, finis chapter 7
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02072C9-A235-4140-9F14-BA934604754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F426AB9F-0F73-4CED-8D70-08DC3BB53921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,7 +335,7 @@
     <t>Tsempring, rajoitteet kytketyissä kappaleissa</t>
   </si>
   <si>
-    <t>12.00-13.00, 16.45-17.45,</t>
+    <t>12.00-13.00, 16.45-17.45, 18.30-19.30,</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1062,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
Cloth constructor for immediate & secondary neighbors
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9965F5C-9792-4880-BA5B-F1BED1542C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5220F81F-DDFF-4BB8-AC2C-1DE3061264AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2170" yWindow="2080" windowWidth="21600" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
     <t>Kangassimulaatio</t>
   </si>
   <si>
-    <t>11.30-12.30</t>
+    <t>11.30-12.30, 13.00-13.30, 14.15-</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1085,11 +1085,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C21" s="2" t="s">

</xml_diff>

<commit_message>
Some scene stuff for cloth, stuck on how to render
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5220F81F-DDFF-4BB8-AC2C-1DE3061264AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD9D979-5850-4612-90F9-B2B6B60CD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2170" yWindow="2080" windowWidth="21600" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
     <t>Kangassimulaatio</t>
   </si>
   <si>
-    <t>11.30-12.30, 13.00-13.30, 14.15-</t>
+    <t>11.30-12.30, 13.00-13.30, 14.15-16.45</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Finishing up cloth sim
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD9D979-5850-4612-90F9-B2B6B60CD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB9756E-90C4-4793-9892-F5FF09A6ECB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2170" yWindow="2080" windowWidth="21600" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +736,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1094,6 +1094,9 @@
       </c>
       <c r="C21" s="2" t="s">
         <v>101</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sensible defaults for cloth, still update erronous
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB9756E-90C4-4793-9892-F5FF09A6ECB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A25AE3E-846A-4250-AC92-DC223EE67291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2170" yWindow="2080" windowWidth="21600" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2170" yWindow="2080" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>PVM</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>11.30-12.30, 13.00-13.30, 14.15-16.45</t>
+  </si>
+  <si>
+    <t>2 marras</t>
+  </si>
+  <si>
+    <t>18.45-22.15</t>
+  </si>
+  <si>
+    <t>Hyvin taas opittu c++ kummallisuuksia ja linkkerinkin toimintaa. Ihan hyvä meno tuon demonkin kanssa, huomenna se toimi (:</t>
+  </si>
+  <si>
+    <t>Juujuu, tällaista se on kun ei tiedä mitä ei tiedä ja tutoriaalikoodia modernisoiden kompastellaan.</t>
+  </si>
+  <si>
+    <t>Puolivälipaniikki?</t>
   </si>
 </sst>
 </file>
@@ -671,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +751,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>59</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1097,6 +1112,29 @@
       </c>
       <c r="G21">
         <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wind defaults, fixing flag anchoring
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A25AE3E-846A-4250-AC92-DC223EE67291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED3CD43-4465-4FBC-AA7E-1250BC770F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2170" yWindow="2080" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
   <si>
     <t>PVM</t>
   </si>
@@ -360,6 +360,18 @@
   </si>
   <si>
     <t>Puolivälipaniikki?</t>
+  </si>
+  <si>
+    <t>4 marras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kangassimulaation numeerisen epästabiiliuden selvittely, </t>
+  </si>
+  <si>
+    <t>18.00-18.45</t>
+  </si>
+  <si>
+    <t>Merkkivirhe söi miestä liian monta tuntia tässä vaiheessa tutkintoa.</t>
   </si>
 </sst>
 </file>
@@ -686,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1137,6 +1149,20 @@
         <v>3.5</v>
       </c>
     </row>
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
more matrix operations implemented, inverse, transpose, determinant for 3x4
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AC0E77-A519-488E-86EF-E70C0A20311A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0A684A-1FB8-41D2-9278-4B2907196CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3150" yWindow="2390" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>PVM</t>
   </si>
@@ -368,9 +368,6 @@
     <t>17.15-20.15</t>
   </si>
   <si>
-    <t>"The Mathematics of Rotations", oppikirjasta 145-169</t>
-  </si>
-  <si>
     <t>Kangassimulaation numeerisen epästabiiliuden selvittely, oppikirjaa eteenpäin 133-143</t>
   </si>
   <si>
@@ -396,6 +393,18 @@
   </si>
   <si>
     <t>Tunnin verran vietetty aikaa kvaternionien parissa, kyllä jotakin jäi käteen mutta jos kysyt osaanko selittää niin tokkopa. Matriisikertailut huomisen heiniä, tänään opiskeltiin uutta.</t>
+  </si>
+  <si>
+    <t>6 marras</t>
+  </si>
+  <si>
+    <t>"The Mathematics of Rotations", oppikirjasta 145-161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oppikirjasta 162- , Implementing mathematics of rotations, </t>
+  </si>
+  <si>
+    <t>9.15-11.15, 12:15</t>
   </si>
 </sst>
 </file>
@@ -722,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,7 +796,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>68</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1090,7 +1099,7 @@
         <v>88</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>89</v>
@@ -1130,7 +1139,7 @@
         <v>97</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -1144,7 +1153,7 @@
         <v>99</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21">
         <v>4</v>
@@ -1158,7 +1167,7 @@
         <v>101</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>103</v>
@@ -1181,10 +1190,10 @@
         <v>106</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>107</v>
@@ -1201,19 +1210,33 @@
         <v>109</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="G24">
         <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished updating math library for rigid bodies
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0A684A-1FB8-41D2-9278-4B2907196CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB05F3-A532-46F9-8E17-C6967D15D4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3150" yWindow="2390" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>PVM</t>
   </si>
@@ -401,10 +401,16 @@
     <t>"The Mathematics of Rotations", oppikirjasta 145-161</t>
   </si>
   <si>
-    <t xml:space="preserve">oppikirjasta 162- , Implementing mathematics of rotations, </t>
-  </si>
-  <si>
-    <t>9.15-11.15, 12:15</t>
+    <t xml:space="preserve">oppikirjasta 162-192 , Implementing mathematics of rotations, </t>
+  </si>
+  <si>
+    <t>9.15-11.15, 12:15-14.15</t>
+  </si>
+  <si>
+    <t>Tuhti päivä, osa kaavoista kirjoitettiin itse. Kvaternin kohdalla luovutin.</t>
+  </si>
+  <si>
+    <t>Aaltoillen, asia oli tuttua mutta uuttakin tuli sopivassa suhteessa. Yritin painottaa etenemistä.</t>
   </si>
 </sst>
 </file>
@@ -733,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,7 +802,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>71.5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1225,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -1235,8 +1241,14 @@
       <c r="C25" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="G25">
-        <v>3.5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rigidbody ready for integration next - needs propably accessors and mutators and some cleanup
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EF46A7-7DF5-4DBF-9548-5F8581F4128A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9580F6-B5CC-4F5A-9850-325CCFC01F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="2790" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,10 +416,10 @@
     <t>Muutaman tunnin verran vietetty aikaa kvaternionien parissa, kyllä jotakin jäi käteen mutta jos kysyt osaanko selittää niin tokkopa. Matriisikertailut huomisen heiniä, tänään opiskeltiin uutta.</t>
   </si>
   <si>
-    <t>12.45-14.15,</t>
-  </si>
-  <si>
     <t>Kovat kappaleet, s.194-212</t>
+  </si>
+  <si>
+    <t>12.45-14.45</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>73.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1265,13 +1265,13 @@
         <v>123</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="G26">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rigidbody integration and scaffolding in place. Next week demos
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9580F6-B5CC-4F5A-9850-325CCFC01F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA626D16-7026-4B7F-A771-FE8CD8799BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="2790" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>PVM</t>
   </si>
@@ -416,10 +416,16 @@
     <t>Muutaman tunnin verran vietetty aikaa kvaternionien parissa, kyllä jotakin jäi käteen mutta jos kysyt osaanko selittää niin tokkopa. Matriisikertailut huomisen heiniä, tänään opiskeltiin uutta.</t>
   </si>
   <si>
-    <t>Kovat kappaleet, s.194-212</t>
-  </si>
-  <si>
-    <t>12.45-14.45</t>
+    <t>12.45-14.45, 15.45-16.15</t>
+  </si>
+  <si>
+    <t>Ihan Jees, suht simppelisti rakentuu sen partikkelijärjestelmän päälle. Katsotaan vielä ensi viikolla mitä jäi käteen teoriatankkauksesta ja täydennetään aukkoja tekemällä demo.</t>
+  </si>
+  <si>
+    <t>Partikkeleilleko voisi siis saada vesisimun aikaan? Voisi olla hyvä niitä kypsytellä vielä kun kirjasta alkaa olla enemmän takana kuin edessä.</t>
+  </si>
+  <si>
+    <t>Kovat kappaleet, s.194-213 luku 10.</t>
   </si>
 </sst>
 </file>
@@ -748,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,7 +817,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>74</v>
+        <v>74.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1260,18 +1266,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>126</v>
+      <c r="F26" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some rigidbody test scene scaffolding
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA626D16-7026-4B7F-A771-FE8CD8799BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078EA7CC-AE6C-4A62-82D7-05F6595B1580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="2790" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>PVM</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>Kovat kappaleet, s.194-213 luku 10.</t>
+  </si>
+  <si>
+    <t>10 marras</t>
+  </si>
+  <si>
+    <t>Kovien kappaleiden demon aloitus</t>
   </si>
 </sst>
 </file>
@@ -752,9 +758,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1286,6 +1292,17 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added registry for rigid body affecting forces, similar to particles
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078EA7CC-AE6C-4A62-82D7-05F6595B1580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1C8B79-FC03-494A-98BF-C7DC87FC6CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="2790" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>PVM</t>
   </si>
@@ -432,6 +432,24 @@
   </si>
   <si>
     <t>Kovien kappaleiden demon aloitus</t>
+  </si>
+  <si>
+    <t>18.00-20.00</t>
+  </si>
+  <si>
+    <t>Vähän maanantai ja heikot unet alla pitkän päivän iltana, mutta ehk siitä jotain jäi käteen. Erityisesti kiinnostaa katsoa ymmärsinkö kaiken oleellisen mallintaakseni seuraavaa demoa.</t>
+  </si>
+  <si>
+    <t>Tässähän alkaa tätä teknistä velkaakin jo olla, ehkä sitten kurssin loppupuolella katsellaan jos jää aikaa.</t>
+  </si>
+  <si>
+    <t>12 marras</t>
+  </si>
+  <si>
+    <t>14.00-16.00</t>
+  </si>
+  <si>
+    <t>Kovien kappaleiden demo</t>
   </si>
 </sst>
 </file>
@@ -758,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -823,7 +841,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>74.5</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1292,15 +1310,38 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="5">
-        <v>0.75</v>
+      <c r="B27" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>131</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed redundant operations around update on mobile scene
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1C8B79-FC03-494A-98BF-C7DC87FC6CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202B94FA-8D9F-425F-86AA-163CA5C8B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="2790" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="2850" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,9 +419,6 @@
     <t>12.45-14.45, 15.45-16.15</t>
   </si>
   <si>
-    <t>Ihan Jees, suht simppelisti rakentuu sen partikkelijärjestelmän päälle. Katsotaan vielä ensi viikolla mitä jäi käteen teoriatankkauksesta ja täydennetään aukkoja tekemällä demo.</t>
-  </si>
-  <si>
     <t>Partikkeleilleko voisi siis saada vesisimun aikaan? Voisi olla hyvä niitä kypsytellä vielä kun kirjasta alkaa olla enemmän takana kuin edessä.</t>
   </si>
   <si>
@@ -450,6 +447,9 @@
   </si>
   <si>
     <t>Kovien kappaleiden demo</t>
+  </si>
+  <si>
+    <t>Ihan Jees, suht simppelisti rakentuu sen partikkelijärjestelmän päälle, tai ainakin periaatteet on samoja. Katsotaan vielä ensi viikolla mitä jäi käteen teoriatankkauksesta ja täydennetään aukkoja tekemällä demo.</t>
   </si>
 </sst>
 </file>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1298,13 +1298,13 @@
         <v>126</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="G26">
         <v>2.5</v>
@@ -1312,19 +1312,19 @@
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="D27" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="G27">
         <v>2</v>
@@ -1332,13 +1332,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="G28">
         <v>2</v>

</xml_diff>

<commit_message>
Investigating not integrating mobile scene
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202B94FA-8D9F-425F-86AA-163CA5C8B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734AF74C-3832-4696-99C4-486E7D8F56AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="2850" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6650" yWindow="3360" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>PVM</t>
   </si>
@@ -443,13 +443,16 @@
     <t>12 marras</t>
   </si>
   <si>
-    <t>14.00-16.00</t>
-  </si>
-  <si>
     <t>Kovien kappaleiden demo</t>
   </si>
   <si>
     <t>Ihan Jees, suht simppelisti rakentuu sen partikkelijärjestelmän päälle, tai ainakin periaatteet on samoja. Katsotaan vielä ensi viikolla mitä jäi käteen teoriatankkauksesta ja täydennetään aukkoja tekemällä demo.</t>
+  </si>
+  <si>
+    <t>Ihan hyvä meininki, tässsä se ymmärrys karttuu kun korjaa virheitä.</t>
+  </si>
+  <si>
+    <t>14.00-16.00, 17.45-18.45, 19.00-</t>
   </si>
 </sst>
 </file>
@@ -778,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,7 +844,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>78.5</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1301,7 +1304,7 @@
         <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>127</v>
@@ -1330,18 +1333,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>134</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>136</v>
+      <c r="D28" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inverseInertiaTensor worldspace stuff
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734AF74C-3832-4696-99C4-486E7D8F56AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D120535-DFB2-44B9-9305-7F0E6FA88B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6650" yWindow="3360" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
     <t>Ihan hyvä meininki, tässsä se ymmärrys karttuu kun korjaa virheitä.</t>
   </si>
   <si>
-    <t>14.00-16.00, 17.45-18.45, 19.00-</t>
+    <t>14.00-16.00, 17.45-18.45, 19.00-20.00</t>
   </si>
 </sst>
 </file>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -844,7 +844,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>79.5</v>
+        <v>80.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1347,7 +1347,7 @@
         <v>137</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating rope scene for a change of pace
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D120535-DFB2-44B9-9305-7F0E6FA88B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5351DE-B76B-4884-B120-571A8C1E8DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6650" yWindow="3360" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>PVM</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>14.00-16.00, 17.45-18.45, 19.00-20.00</t>
+  </si>
+  <si>
+    <t>Huomaa tässä, että aika paljon jäi sisäistämättä tuosta opitusta kun virheen etsimisen kanssa menee sormi suuhun.</t>
   </si>
 </sst>
 </file>
@@ -782,7 +785,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1333,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -1345,6 +1348,9 @@
       </c>
       <c r="D28" s="2" t="s">
         <v>137</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="G28">
         <v>4</v>

</xml_diff>

<commit_message>
Kick now pleasantly working, next debug line
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5351DE-B76B-4884-B120-571A8C1E8DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC3F546-CD9E-4C68-BB05-9889152471E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6650" yWindow="3360" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5950" yWindow="7160" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>PVM</t>
   </si>
@@ -456,6 +456,15 @@
   </si>
   <si>
     <t>Huomaa tässä, että aika paljon jäi sisäistämättä tuosta opitusta kun virheen etsimisen kanssa menee sormi suuhun.</t>
+  </si>
+  <si>
+    <t>13 marras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Köysidemon parantelua, </t>
+  </si>
+  <si>
+    <t>10.00-11.30, 12.00-12.30</t>
   </si>
 </sst>
 </file>
@@ -782,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,6 +1365,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on line utility
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC3F546-CD9E-4C68-BB05-9889152471E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A193924-9023-4F0D-8449-F47CBEC15A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5950" yWindow="7160" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,9 +449,6 @@
     <t>Ihan Jees, suht simppelisti rakentuu sen partikkelijärjestelmän päälle, tai ainakin periaatteet on samoja. Katsotaan vielä ensi viikolla mitä jäi käteen teoriatankkauksesta ja täydennetään aukkoja tekemällä demo.</t>
   </si>
   <si>
-    <t>Ihan hyvä meininki, tässsä se ymmärrys karttuu kun korjaa virheitä.</t>
-  </si>
-  <si>
     <t>14.00-16.00, 17.45-18.45, 19.00-20.00</t>
   </si>
   <si>
@@ -461,10 +458,13 @@
     <t>13 marras</t>
   </si>
   <si>
-    <t xml:space="preserve">Köysidemon parantelua, </t>
-  </si>
-  <si>
-    <t>10.00-11.30, 12.00-12.30</t>
+    <t>Köysidemon parantelua, kovien kappaleiden demon debug</t>
+  </si>
+  <si>
+    <t>Ihan hyvä meininki, tässsä se ymmärrys karttuu kun korjaa virheitä. Integrate ei toimi, jotakin on varmaan jäänyt alustamatta.</t>
+  </si>
+  <si>
+    <t>10.00-11.30, 12.00-12.30, 14.00-</t>
   </si>
 </sst>
 </file>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1350,16 +1350,16 @@
         <v>134</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>135</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G28">
         <v>4</v>
@@ -1367,13 +1367,13 @@
     </row>
     <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized some stuff in rope, kick works nicely
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A193924-9023-4F0D-8449-F47CBEC15A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC75EE2-D6C9-4270-9615-9188D69C8508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5950" yWindow="7160" windowWidth="27420" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
     <t>Ihan hyvä meininki, tässsä se ymmärrys karttuu kun korjaa virheitä. Integrate ei toimi, jotakin on varmaan jäänyt alustamatta.</t>
   </si>
   <si>
-    <t>10.00-11.30, 12.00-12.30, 14.00-</t>
+    <t>10.00-11.30, 12.00-12.30, 14.00-16.30</t>
   </si>
 </sst>
 </file>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,7 +856,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>80.5</v>
+        <v>84.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1374,6 +1374,9 @@
       </c>
       <c r="C29" s="2" t="s">
         <v>140</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cant find bug, added vector3 debug print util
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5FF1ED-3B6F-4190-A6EC-7B288FF3B4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE922E7E-AD48-4207-92D1-269175774B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="7400" windowWidth="25440" windowHeight="12530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
     <t>Ihan hyvä meininki, tässsä se ymmärrys karttuu kun korjaa virheitä. Integrate ei toimi, jotakin on varmaan jäänyt alustamatta.</t>
   </si>
   <si>
-    <t>10.00-11.30, 12.00-12.30, 14.00-18.00, 19.00-</t>
+    <t>10.00-11.30, 12.00-12.30, 14.00-18.00, 19.00-20.00</t>
   </si>
 </sst>
 </file>
@@ -794,7 +794,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Coordinate mismatch fixed, local vs world space misunderstanding
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE922E7E-AD48-4207-92D1-269175774B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83AFFF5-5B93-4ED6-BCA8-EE09E6C0E37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="7400" windowWidth="25440" windowHeight="12530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,7 +794,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,7 +856,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>86.5</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1376,7 +1376,7 @@
         <v>140</v>
       </c>
       <c r="G29">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed redundant angularvelocity from rigidbody
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83AFFF5-5B93-4ED6-BCA8-EE09E6C0E37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B22E460-43CE-442B-BD5C-697D69E5380F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="7400" windowWidth="25440" windowHeight="12530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3090" yWindow="2260" windowWidth="25340" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>PVM</t>
   </si>
@@ -465,6 +465,15 @@
   </si>
   <si>
     <t>10.00-11.30, 12.00-12.30, 14.00-18.00, 19.00-20.00</t>
+  </si>
+  <si>
+    <t>14 marras</t>
+  </si>
+  <si>
+    <t>8.45-11.15, 12.00-13.00</t>
+  </si>
+  <si>
+    <t>Kovien kappaleiden demon debug, tsemppi</t>
   </si>
 </sst>
 </file>
@@ -791,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,7 +865,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>87.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1377,6 +1386,20 @@
       </c>
       <c r="G29">
         <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Succesful small refactor introducing polymorphism and generic mesh
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B22E460-43CE-442B-BD5C-697D69E5380F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2AD792-F69C-43BA-A64D-3FC67E891504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3090" yWindow="2260" windowWidth="25340" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>PVM</t>
   </si>
@@ -474,6 +474,18 @@
   </si>
   <si>
     <t>Kovien kappaleiden demon debug, tsemppi</t>
+  </si>
+  <si>
+    <t>17 marras</t>
+  </si>
+  <si>
+    <t>Oppikirjasta 213-228(kertaus), 231-</t>
+  </si>
+  <si>
+    <t>10.30-11.00, 12.15-</t>
+  </si>
+  <si>
+    <t>Rigidbody moottorikoodin kokonaisuuden kertausvilkuilu ( tässä kohtaa ei tehdä perässä uutta demoa näistä, vaan tehdään sitten kun on törmäykset), johdanto törmäyksiin kovilla kappaleilla, renderer/utility kirjaston päivitystä</t>
   </si>
 </sst>
 </file>
@@ -800,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1398,8 +1410,23 @@
       <c r="C30" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="F30" s="2"/>
       <c r="G30">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed tech debt in rope scene with proper raycast
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2AD792-F69C-43BA-A64D-3FC67E891504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BBD4E8-C03A-414F-ADA8-B36C0C26B924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3090" yWindow="2260" windowWidth="25340" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,10 +482,10 @@
     <t>Oppikirjasta 213-228(kertaus), 231-</t>
   </si>
   <si>
-    <t>10.30-11.00, 12.15-</t>
-  </si>
-  <si>
     <t>Rigidbody moottorikoodin kokonaisuuden kertausvilkuilu ( tässä kohtaa ei tehdä perässä uutta demoa näistä, vaan tehdään sitten kun on törmäykset), johdanto törmäyksiin kovilla kappaleilla, renderer/utility kirjaston päivitystä</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12.15-14.45,</t>
   </si>
 </sst>
 </file>
@@ -877,7 +877,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>91</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1420,13 +1420,16 @@
         <v>146</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>147</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+      <c r="G31">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some foldering + update include paths
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BBD4E8-C03A-414F-ADA8-B36C0C26B924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6DA84A-9D82-4FD9-A426-C2ACB02C4C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="2260" windowWidth="25340" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="1840" windowWidth="25220" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,13 +479,13 @@
     <t>17 marras</t>
   </si>
   <si>
-    <t>Oppikirjasta 213-228(kertaus), 231-</t>
-  </si>
-  <si>
-    <t>Rigidbody moottorikoodin kokonaisuuden kertausvilkuilu ( tässä kohtaa ei tehdä perässä uutta demoa näistä, vaan tehdään sitten kun on törmäykset), johdanto törmäyksiin kovilla kappaleilla, renderer/utility kirjaston päivitystä</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 12.15-14.45,</t>
+  </si>
+  <si>
+    <t>Rigidbody moottorikoodin kokonaisuuden kertausvilkuilu ( tässä kohtaa ei tehdä perässä uutta demoa näistä, vaan tehdään sitten kun on törmäykset), johdanto törmäyksiin kovilla kappaleilla, renderer/utility kirjaston päivitystä, ropescene teknisen velan poisto</t>
+  </si>
+  <si>
+    <t>Oppikirjasta 213-228(kertaus)</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1415,15 +1415,15 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>146</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
deletion of node from hierarchy / destructor
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6DA84A-9D82-4FD9-A426-C2ACB02C4C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E8F8B0-C8A2-45C3-AD85-A45E57970D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1840" windowWidth="25220" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>PVM</t>
   </si>
@@ -482,10 +482,22 @@
     <t xml:space="preserve"> 12.15-14.45,</t>
   </si>
   <si>
-    <t>Rigidbody moottorikoodin kokonaisuuden kertausvilkuilu ( tässä kohtaa ei tehdä perässä uutta demoa näistä, vaan tehdään sitten kun on törmäykset), johdanto törmäyksiin kovilla kappaleilla, renderer/utility kirjaston päivitystä, ropescene teknisen velan poisto</t>
-  </si>
-  <si>
-    <t>Oppikirjasta 213-228(kertaus)</t>
+    <t>18 marras</t>
+  </si>
+  <si>
+    <t>Oppikirjasta 213-228(kertaus),renderer/utility kirjaston päivitystä, ropescene teknisen velan poisto</t>
+  </si>
+  <si>
+    <t>18.45-20.45</t>
+  </si>
+  <si>
+    <t>Oppikirjasta 231-249, Rajaava voluumipuu, rajaava pallo, ja rajaavaan rakenteeseen lisääminen</t>
+  </si>
+  <si>
+    <t>Nyt tuli aika paljon uutta kamaa ja mitä ihmettä täällä näitä templateja alettiin viljelemään. Täytyy pysähdellä ja selvitellä.</t>
+  </si>
+  <si>
+    <t>Pikku siistimistä. Haluan katsoa tämän collision pyräyksen innoittamana nyt sitten onnistuisiko vaihtaa esimerkiksi siihen kasipuuksi alla oleva tietorakenne, ja miten iso aikapanostusta vaatisi. Ei ehkä kurssin aikana.</t>
   </si>
 </sst>
 </file>
@@ -812,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -877,7 +889,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>93.5</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1415,7 +1427,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -1425,11 +1437,29 @@
       <c r="C31" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>148</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="G31">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filling out the contact classes
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E8F8B0-C8A2-45C3-AD85-A45E57970D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1908E1-7BEC-4508-80C1-1BA3C17D54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>PVM</t>
   </si>
@@ -498,6 +498,15 @@
   </si>
   <si>
     <t>Pikku siistimistä. Haluan katsoa tämän collision pyräyksen innoittamana nyt sitten onnistuisiko vaihtaa esimerkiksi siihen kasipuuksi alla oleva tietorakenne, ja miten iso aikapanostusta vaatisi. Ei ehkä kurssin aikana.</t>
+  </si>
+  <si>
+    <t>19 marras</t>
+  </si>
+  <si>
+    <t>16.30-17.30</t>
+  </si>
+  <si>
+    <t>Rajaavasta rakenteesta poistaminen. Nopea johdanto partiotioiviin rakenteisiin.</t>
   </si>
 </sst>
 </file>
@@ -824,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1462,6 +1471,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="33" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
collision detection algorithm for two spheres
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1908E1-7BEC-4508-80C1-1BA3C17D54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A48439-2445-425E-820F-B3391BC5DC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,16 +497,16 @@
     <t>Nyt tuli aika paljon uutta kamaa ja mitä ihmettä täällä näitä templateja alettiin viljelemään. Täytyy pysähdellä ja selvitellä.</t>
   </si>
   <si>
-    <t>Pikku siistimistä. Haluan katsoa tämän collision pyräyksen innoittamana nyt sitten onnistuisiko vaihtaa esimerkiksi siihen kasipuuksi alla oleva tietorakenne, ja miten iso aikapanostusta vaatisi. Ei ehkä kurssin aikana.</t>
-  </si>
-  <si>
     <t>19 marras</t>
   </si>
   <si>
-    <t>16.30-17.30</t>
-  </si>
-  <si>
-    <t>Rajaavasta rakenteesta poistaminen. Nopea johdanto partiotioiviin rakenteisiin.</t>
+    <t>16.30-17.30, 18.00-19.00</t>
+  </si>
+  <si>
+    <t>Pikku siistimistä. Haluan katsoa tämän collision pyräyksen innoittamana nyt sitten onnistuisiko vaihtaa esimerkiksi siihen kasipuuksi alla oleva tietorakenne, ja miten iso aikapanostusta vaatisi. Ei ehkä kurssin aikana, ja muutenkin tässä tulee kyllä uutta vielä aika reippaasti tulevina tunteina. Katsotaan mihin riittää aika ja energia.</t>
+  </si>
+  <si>
+    <t>Rajaavasta rakenteesta poistaminen, nopea johdanto partiotiointirakenteisiin ja Törmäystarkastelun ABC:tä millingtonin kanssa. Pääsin kahden pallon törmäykseen, s 249-279.</t>
   </si>
 </sst>
 </file>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,7 +898,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>95.5</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1451,7 +1451,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -1465,21 +1465,24 @@
         <v>152</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>156</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
two box intersection test
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A48439-2445-425E-820F-B3391BC5DC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA95261-1926-41F8-8977-7A0A9DBB07D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t>PVM</t>
   </si>
@@ -507,6 +507,12 @@
   </si>
   <si>
     <t>Rajaavasta rakenteesta poistaminen, nopea johdanto partiotiointirakenteisiin ja Törmäystarkastelun ABC:tä millingtonin kanssa. Pääsin kahden pallon törmäykseen, s 249-279.</t>
+  </si>
+  <si>
+    <t>23 marras</t>
+  </si>
+  <si>
+    <t>Erottavan hypertason teoreema, kahden monikulmion leikkaustarkastelu,</t>
   </si>
 </sst>
 </file>
@@ -833,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1485,6 +1491,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="34" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Box plane + box point collision algos
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA95261-1926-41F8-8977-7A0A9DBB07D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A659CFCA-7C61-4553-A949-A8470F0EE9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>PVM</t>
   </si>
@@ -512,7 +512,22 @@
     <t>23 marras</t>
   </si>
   <si>
-    <t>Erottavan hypertason teoreema, kahden monikulmion leikkaustarkastelu,</t>
+    <t>18.30-20.30</t>
+  </si>
+  <si>
+    <t>Paljon taas teoriaa tankattu, mutta ehkä se tästä sitte pikkuhiljaa maturoituu</t>
+  </si>
+  <si>
+    <t>Vaatii uudelleenlukemista, mutta virkeänä ja valppaana keskittyneesti eteenpäin, pieniä sivupolkuja unohtamatta.</t>
+  </si>
+  <si>
+    <t>26 marras</t>
+  </si>
+  <si>
+    <t>Siirtyminen törmäyksen havaitsemisesta kontaktien aiheuttamiin voimiin</t>
+  </si>
+  <si>
+    <t>Erottavan hypertason teoreema, kahden monikulmion leikkaustarkastelu (box-box intersection), monikulmion laajennusta, s. 279-290</t>
   </si>
 </sst>
 </file>
@@ -839,7 +854,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
@@ -904,7 +919,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>97.5</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1491,15 +1506,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="5">
-        <v>0.77083333333333337</v>
+      <c r="B34" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filling out some helpers for box box coll
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A659CFCA-7C61-4553-A949-A8470F0EE9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF2D845-1AA0-4051-93EA-2A1DF1390817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>PVM</t>
   </si>
@@ -524,10 +524,13 @@
     <t>26 marras</t>
   </si>
   <si>
-    <t>Siirtyminen törmäyksen havaitsemisesta kontaktien aiheuttamiin voimiin</t>
-  </si>
-  <si>
     <t>Erottavan hypertason teoreema, kahden monikulmion leikkaustarkastelu (box-box intersection), monikulmion laajennusta, s. 279-290</t>
+  </si>
+  <si>
+    <t>9.30-11.30</t>
+  </si>
+  <si>
+    <t>Siirtyminen törmäyksen havaitsemisesta kontaktien aiheuttamiin voimiin, Kahden laatikon törmäystarkastelu, laatikon ja tason, ja laatikon ja pisteen törmäystarkastelu</t>
   </si>
 </sst>
 </file>
@@ -857,7 +860,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,7 +922,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>99.5</v>
+        <v>101.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1514,7 +1517,7 @@
         <v>158</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>160</v>
@@ -1526,15 +1529,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>161</v>
       </c>
-      <c r="B35" s="5">
-        <v>0.39583333333333331</v>
+      <c r="B35" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to modernize the helpers as well
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF2D845-1AA0-4051-93EA-2A1DF1390817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E8C5E9-5481-449E-A425-D9A86C46CCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9870" yWindow="4000" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9920" yWindow="4010" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,10 +527,10 @@
     <t>Erottavan hypertason teoreema, kahden monikulmion leikkaustarkastelu (box-box intersection), monikulmion laajennusta, s. 279-290</t>
   </si>
   <si>
-    <t>9.30-11.30</t>
-  </si>
-  <si>
-    <t>Siirtyminen törmäyksen havaitsemisesta kontaktien aiheuttamiin voimiin, Kahden laatikon törmäystarkastelu, laatikon ja tason, ja laatikon ja pisteen törmäystarkastelu</t>
+    <t>Laatikon ja tason, ja laatikon ja pisteen törmäystarkastelu,  Kahden laatikon törmäystarkastelu, kertailua ja uudelleenlukemista</t>
+  </si>
+  <si>
+    <t>9.30-11.30, 12.00-13.30, 18.15-</t>
   </si>
 </sst>
 </file>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>101.5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1529,18 +1529,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>161</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="G35">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Box box collision algorithm naive implementation
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E8C5E9-5481-449E-A425-D9A86C46CCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75B292F-881A-4CD7-83C4-957E6C75FE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9920" yWindow="4010" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,7 +530,7 @@
     <t>Laatikon ja tason, ja laatikon ja pisteen törmäystarkastelu,  Kahden laatikon törmäystarkastelu, kertailua ja uudelleenlukemista</t>
   </si>
   <si>
-    <t>9.30-11.30, 12.00-13.30, 18.15-</t>
+    <t>9.30-11.30, 12.00-13.30, 18.15-19.15,</t>
   </si>
 </sst>
 </file>
@@ -860,7 +860,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Contact basis calculation + qol helper
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75B292F-881A-4CD7-83C4-957E6C75FE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58754CB4-285A-4D5B-8A38-0C58B08735D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9920" yWindow="4010" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>PVM</t>
   </si>
@@ -530,7 +530,16 @@
     <t>Laatikon ja tason, ja laatikon ja pisteen törmäystarkastelu,  Kahden laatikon törmäystarkastelu, kertailua ja uudelleenlukemista</t>
   </si>
   <si>
-    <t>9.30-11.30, 12.00-13.30, 18.15-19.15,</t>
+    <t>9.30-11.30, 12.00-13.30, 18.15-19.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ihan jees meininki, ei valittamista. Hirveästi uutta teoriasisältöä ei ollut, nyt lähinä aiempien päivien sulattelua ja työstämistä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hieman modernisoitua tuli taas millingtonin koodia, ja gitin kanssa huolellisuutta opeteltua. Kohti ammattimaista versionhallintaa. </t>
+  </si>
+  <si>
+    <t>Koodikanta ihan OK mallilla jättää törmäystarkastelut sikseen, siirrytään kontaktin generoiviin voimiin.</t>
   </si>
 </sst>
 </file>
@@ -859,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -922,7 +931,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>103</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1539,8 +1548,17 @@
       <c r="C35" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="D35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" t="s">
+        <v>167</v>
+      </c>
       <c r="G35">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Happy for now to tutorial progres
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58754CB4-285A-4D5B-8A38-0C58B08735D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72669F4C-7131-4CF1-9246-5B412FF9AA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="4010" windowWidth="21980" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8280" yWindow="2420" windowWidth="23620" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>PVM</t>
   </si>
@@ -540,6 +540,21 @@
   </si>
   <si>
     <t>Koodikanta ihan OK mallilla jättää törmäystarkastelut sikseen, siirrytään kontaktin generoiviin voimiin.</t>
+  </si>
+  <si>
+    <t>27 marras</t>
+  </si>
+  <si>
+    <t>18.00-20.45,21.15-22.00</t>
+  </si>
+  <si>
+    <t>Vähän copy pasteksi loppupuolella meni. Pikkuhiljaa palastellaan eteenpäin samalla kun tehdään demoa, halusin käydä teorian nyt hieman ripeämmin jotta ehtii saada demon aikaiseksi kurssilla ja saa koodin kääntymään. Oppivelkaa kasvatettu kyllä, mutta eipä se suurimmalta osin mahdottomaltakaan tuntunut.</t>
+  </si>
+  <si>
+    <t>Törmäysfysiikkaa, törmäysten aiheuttamat voimat. 301-350</t>
+  </si>
+  <si>
+    <t>Kirjasta kahlattu oleellisimmat asiat, nyt lueskellaan rauhallisempaan tahtiin relevantteja asioita hieman mitä ehtii. Kurssi alkaa olla loppusuoralla oppisisältötavoitteellisesti, nyt vikat demot pakettiin ja pientä koodikannan siisitimistä ja artikkelin etsintää.</t>
   </si>
 </sst>
 </file>
@@ -866,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,7 +946,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>104.5</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1559,6 +1574,26 @@
       </c>
       <c r="G35">
         <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some scaffolding for tomorrows work
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72669F4C-7131-4CF1-9246-5B412FF9AA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A52C38-D5EB-4BC6-95F2-51E6F5567B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="2420" windowWidth="23620" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15516" yWindow="9756" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>PVM</t>
   </si>
@@ -555,6 +555,15 @@
   </si>
   <si>
     <t>Kirjasta kahlattu oleellisimmat asiat, nyt lueskellaan rauhallisempaan tahtiin relevantteja asioita hieman mitä ehtii. Kurssi alkaa olla loppusuoralla oppisisältötavoitteellisesti, nyt vikat demot pakettiin ja pientä koodikannan siisitimistä ja artikkelin etsintää.</t>
+  </si>
+  <si>
+    <t>28 marras</t>
+  </si>
+  <si>
+    <t>12.00-13.30, 19.15-20.15</t>
+  </si>
+  <si>
+    <t>Tsemppirinki, Millingtonin törmäysdemon pohjakoodiin tutustumista</t>
   </si>
 </sst>
 </file>
@@ -881,25 +890,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" customWidth="1"/>
-    <col min="4" max="4" width="41.453125" customWidth="1"/>
-    <col min="5" max="5" width="34.54296875" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -946,10 +955,10 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -969,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -989,7 +998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="216" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1135,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1155,7 +1164,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1175,7 +1184,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1195,7 +1204,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1241,7 +1250,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -1295,7 +1304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -1395,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -1415,7 +1424,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -1435,7 +1444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -1455,7 +1464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -1484,7 +1493,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>157</v>
       </c>
@@ -1553,7 +1562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -1576,7 +1585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>168</v>
       </c>
@@ -1594,6 +1603,20 @@
       </c>
       <c r="G36">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the box scene, debugging stuff
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953F0236-A01E-44A7-BA74-A88BCB41466F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361DFEEC-0245-4359-908A-192F2B016714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15516" yWindow="9756" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18072" yWindow="7848" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t>PVM</t>
   </si>
@@ -569,7 +569,10 @@
     <t>29 marras</t>
   </si>
   <si>
-    <t>Törmäysdemoa</t>
+    <t>Törmäysdemoa, rigidbody ja  törmäystarkasteluun liittyvien luokkien tutkintaa</t>
+  </si>
+  <si>
+    <t>16.00-18.00, 18.45-21-45</t>
   </si>
 </sst>
 </file>
@@ -899,7 +902,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +964,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>110.5</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1625,15 +1628,18 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>176</v>
       </c>
-      <c r="B38" s="5">
-        <v>0.66666666666666663</v>
+      <c r="B38" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>177</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working naive floor collision
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361DFEEC-0245-4359-908A-192F2B016714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A0DEE-FA91-460F-8178-54CB602E2B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18072" yWindow="7848" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>PVM</t>
   </si>
@@ -573,6 +573,18 @@
   </si>
   <si>
     <t>16.00-18.00, 18.45-21-45</t>
+  </si>
+  <si>
+    <t>1 joulu</t>
+  </si>
+  <si>
+    <t>Samoissa puuhissa jatketaan. Törmäykset(tai ainakin leikkaukset) tunnistetaan.</t>
+  </si>
+  <si>
+    <t>Jatkoa 29 marras</t>
+  </si>
+  <si>
+    <t>9.45-11.15</t>
   </si>
 </sst>
 </file>
@@ -899,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,7 +976,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>115.5</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1640,6 +1652,23 @@
       </c>
       <c r="G38">
         <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G39">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Towards fluids : resting contacts not implemented will prevent box stacking in collision demo
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A0DEE-FA91-460F-8178-54CB602E2B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CC5405-93AA-4D78-A593-31B5D082695B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18072" yWindow="7848" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t>PVM</t>
   </si>
@@ -578,13 +578,25 @@
     <t>1 joulu</t>
   </si>
   <si>
-    <t>Samoissa puuhissa jatketaan. Törmäykset(tai ainakin leikkaukset) tunnistetaan.</t>
-  </si>
-  <si>
-    <t>Jatkoa 29 marras</t>
-  </si>
-  <si>
-    <t>9.45-11.15</t>
+    <t>Jatkoa 29 marras. Törmäykset maan kanssa tapahtuvat nyt hienosti.</t>
+  </si>
+  <si>
+    <t>Samoissa puuhissa jatketaan. Törmäykset(tai ainakin leikkaukset) tunnistetaan. Mahtava meininki iltapäivästä kun törmäykset lähtivät toimimaan. Sitten menikin sormi suhun kahden laatikon törmäyksessä. Sellaista se on.</t>
+  </si>
+  <si>
+    <t>9.45-11.15, 13.15-15.15</t>
+  </si>
+  <si>
+    <t>3 joulu</t>
+  </si>
+  <si>
+    <t>Minimaalisen törmäysdemon ongelmat ratkaistu</t>
+  </si>
+  <si>
+    <t>Kappaleet törmäävät. Nyt enginen on todistettu jollakin tasolla kattavan 4/5 oppimistavoitteesta. Meininki huipussa. Toki, ongelmana oli useamman kappaleen samanaikainen törmääminen. Täytyy pohtia, haluaako käyttää aikaa tähän, vai siirtyäkö fluidisimuun ja tutkimuspaperin etsintään. Törmäyksistä pitäisi varmaan lukea oma kirjansa jossakin vaiheessa, mutta tässä kohtaa ehkä riittää tuo demo. Teen varmaan vielä pikkuisen päivitystä että saan tekstuurit.</t>
+  </si>
+  <si>
+    <t>17.45-20.15</t>
   </si>
 </sst>
 </file>
@@ -911,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,7 +988,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>117</v>
+        <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1654,21 +1666,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>179</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>182</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="F39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="G39">
-        <v>1.5</v>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Investigating compute shader updating + fragment rendering via ssbo. Has a typo/bug
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CC5405-93AA-4D78-A593-31B5D082695B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFCD30A-A2E0-47D6-AF5A-4EE207AADE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7536" yWindow="5724" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>PVM</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>17.45-20.15</t>
+  </si>
+  <si>
+    <t>4 joulu</t>
+  </si>
+  <si>
+    <t>Laskentavarjostimen käyttöönottoa</t>
+  </si>
+  <si>
+    <t>13.00-14.00, 18.00-20.00</t>
   </si>
 </sst>
 </file>
@@ -923,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +997,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>121.5</v>
+        <v>124.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1699,6 +1708,20 @@
       </c>
       <c r="G40">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rendering now working with properly aligned struct
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFCD30A-A2E0-47D6-AF5A-4EE207AADE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C6BFE-63A8-462E-8C26-85CBAFD73096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7536" yWindow="5724" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>PVM</t>
   </si>
@@ -606,6 +606,12 @@
   </si>
   <si>
     <t>13.00-14.00, 18.00-20.00</t>
+  </si>
+  <si>
+    <t>5 joulu</t>
+  </si>
+  <si>
+    <t>Laskentavarjostin scene setup</t>
   </si>
 </sst>
 </file>
@@ -932,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1724,6 +1730,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Oriented & scaled bounding volume to be centered to the scene, debugging its visuals
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C6BFE-63A8-462E-8C26-85CBAFD73096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5290BE5-F99A-4F8A-BC35-E3B549A5B6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7536" yWindow="5724" windowWidth="21024" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7536" yWindow="5724" windowWidth="23484" windowHeight="14448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>PVM</t>
   </si>
@@ -611,7 +611,19 @@
     <t>5 joulu</t>
   </si>
   <si>
-    <t>Laskentavarjostin scene setup</t>
+    <t>Laskentavarjostin scene setup, fluiditutoriaalin läpikatselu ja seuraavien askelmerkkien suunnittelu</t>
+  </si>
+  <si>
+    <t>11.45-13.15</t>
+  </si>
+  <si>
+    <t>8 joulu</t>
+  </si>
+  <si>
+    <t>Fluiditutoriaalin palastelua</t>
+  </si>
+  <si>
+    <t>17.45-18.30,</t>
   </si>
 </sst>
 </file>
@@ -938,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,7 +1015,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>124.5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1730,15 +1742,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>190</v>
       </c>
-      <c r="B42" s="5">
-        <v>0.48958333333333331</v>
+      <c r="B42" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>191</v>
+      </c>
+      <c r="G42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some progress in visualization with one giant blobs
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5290BE5-F99A-4F8A-BC35-E3B549A5B6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6B2310-5F7F-4D11-95BC-46E5CC46D3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7536" yWindow="5724" windowWidth="23484" windowHeight="14448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,10 +620,10 @@
     <t>8 joulu</t>
   </si>
   <si>
-    <t>Fluiditutoriaalin palastelua</t>
-  </si>
-  <si>
-    <t>17.45-18.30,</t>
+    <t>Fluiditutoriaalin palastelua, rajaava voluumi ja alkutoimia</t>
+  </si>
+  <si>
+    <t>17.45-19.45, 20.00-21.00</t>
   </si>
 </sst>
 </file>
@@ -953,7 +953,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1756,7 +1756,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -1765,6 +1765,9 @@
       </c>
       <c r="C43" s="2" t="s">
         <v>194</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A bit hacky mini blod radius for trying out 2D blo´b movement
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6B2310-5F7F-4D11-95BC-46E5CC46D3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4165C-A92F-4990-A22C-0119B43CFA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7536" yWindow="5724" windowWidth="23484" windowHeight="14448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -952,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update documentation w screenshot
fix image

typo

layout update

Fix image final?

Update README.md
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapul\FYSM\Impi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4165C-A92F-4990-A22C-0119B43CFA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8187CF7-B225-42F9-B8DF-C3152B818488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7536" yWindow="5724" windowWidth="23484" windowHeight="14448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
   <si>
     <t>PVM</t>
   </si>
@@ -624,6 +624,39 @@
   </si>
   <si>
     <t>17.45-19.45, 20.00-21.00</t>
+  </si>
+  <si>
+    <t>12 joulu</t>
+  </si>
+  <si>
+    <t>15.00-16.00</t>
+  </si>
+  <si>
+    <t>Viimeinen tsemppirinki</t>
+  </si>
+  <si>
+    <t>15 joulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutkimusartikkelin läpisilmäily, </t>
+  </si>
+  <si>
+    <t>18.30-20.00</t>
+  </si>
+  <si>
+    <t>16 joulu</t>
+  </si>
+  <si>
+    <t>Vähän tällaistahan tämä on, oppii kyllä hyvin uutta mutta tähän olisi pitänyt varata enemmän aikaa.</t>
+  </si>
+  <si>
+    <t>Pääsin paremmin kiinni mikä tilanne oli ennen artikkelia, ja sain pintapuolisen ymmärryksen toisesta artikkelin teesistä. Mielestäni kohtuullinen saavutus 4 tunnin työllä.</t>
+  </si>
+  <si>
+    <t>10.00-11.15, 13.00-13.45, 17.30-18.30</t>
+  </si>
+  <si>
+    <t>Tutkimusartikkelin taustalukujen hieman tarkempi lukeminen, luvut 3-4.0, hieman lukua 4.1. Illalla itsearvio</t>
   </si>
 </sst>
 </file>
@@ -950,25 +983,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
-    <col min="4" max="4" width="41.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -994,7 +1027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1015,10 +1048,10 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(G3:G60)</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1038,7 +1071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1058,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1081,7 +1114,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1104,7 +1137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1127,7 +1160,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1147,7 +1180,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1167,7 +1200,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1181,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1204,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1224,7 +1257,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1244,7 +1277,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1264,7 +1297,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -1287,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1310,7 +1343,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -1327,7 +1360,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1350,7 +1383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -1364,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -1378,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -1401,7 +1434,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -1421,7 +1454,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1444,7 +1477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -1464,7 +1497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -1484,7 +1517,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -1504,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -1524,7 +1557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -1538,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -1553,7 +1586,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -1568,7 +1601,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -1588,7 +1621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -1602,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>157</v>
       </c>
@@ -1622,7 +1655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -1645,7 +1678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>168</v>
       </c>
@@ -1665,7 +1698,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -1679,7 +1712,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>176</v>
       </c>
@@ -1693,7 +1726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>179</v>
       </c>
@@ -1711,7 +1744,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -1728,7 +1761,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>187</v>
       </c>
@@ -1742,7 +1775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>190</v>
       </c>
@@ -1756,7 +1789,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -1768,6 +1801,54 @@
       </c>
       <c r="G43">
         <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>196</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>199</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G46">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>